<commit_message>
Migrar todo a el codigo a ingles  (parcial)
</commit_message>
<xml_diff>
--- a/NomenclaturaNombresAG2.xlsx
+++ b/NomenclaturaNombresAG2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>nodo</t>
   </si>
@@ -97,6 +97,18 @@
   </si>
   <si>
     <t>tbw</t>
+  </si>
+  <si>
+    <t>Arco</t>
+  </si>
+  <si>
+    <t>arc</t>
+  </si>
+  <si>
+    <t>Nodo de servicio</t>
+  </si>
+  <si>
+    <t>broker node</t>
   </si>
 </sst>
 </file>
@@ -431,11 +443,12 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="24" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -511,6 +524,12 @@
       </c>
     </row>
     <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
       <c r="E5" t="s">
         <v>21</v>
       </c>
@@ -519,6 +538,12 @@
       </c>
     </row>
     <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
       <c r="E6" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
adicion en el excel la ruat de ejecucion para la creacion de un OCS
</commit_message>
<xml_diff>
--- a/NomenclaturaNombresAG2.xlsx
+++ b/NomenclaturaNombresAG2.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>nodo</t>
   </si>
@@ -163,14 +163,63 @@
   </si>
   <si>
     <t>tp</t>
+  </si>
+  <si>
+    <t>util.createOCSCircuit</t>
+  </si>
+  <si>
+    <t>gridSimulator.addRequestedCircuit(ocsRoute)</t>
+  </si>
+  <si>
+    <t>source.requestOCSCircuit(ocsRoute, permanent, t)</t>
+  </si>
+  <si>
+    <t>requestOCSCircuit(OCSRoute ocsRoute, boolean permanent, Time time)</t>
+  </si>
+  <si>
+    <t>Util</t>
+  </si>
+  <si>
+    <t>OCSSwitchSender</t>
+  </si>
+  <si>
+    <t>HybridSwitchSender</t>
+  </si>
+  <si>
+    <t>HybridSwitchImpl</t>
+  </si>
+  <si>
+    <t>GridSimulator</t>
+  </si>
+  <si>
+    <t>requestedCircuits.add(route);</t>
+  </si>
+  <si>
+    <t>owner.sendNow(ocsRoute.getSource(), request, time)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -198,11 +247,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -292,7 +343,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -327,7 +377,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -503,20 +552,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -530,7 +579,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -550,7 +599,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -567,7 +616,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -587,7 +636,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -601,7 +650,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -615,7 +664,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -629,7 +678,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -643,7 +692,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -657,7 +706,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -671,7 +720,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -679,7 +728,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -693,24 +742,86 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="24.140625" customWidth="1"/>
+    <col min="2" max="2" width="48.42578125" customWidth="1"/>
+    <col min="3" max="3" width="65.5703125" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="D6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="C7" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="C9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="C12" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>